<commit_message>
"updating for start of final quarter"
</commit_message>
<xml_diff>
--- a/literature/literature_update_final.xlsx
+++ b/literature/literature_update_final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/cijensen_calpoly_edu/Documents/MSQE/GSE_580/GSE-580-project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/cijensen_calpoly_edu/Documents/MSQE/GSE_580/GSE-580-project/literature/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{2946FB2A-71EE-4D66-8EE3-C8A44FDB6146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96C0756A-DEE9-4640-BFA5-1010659F6E34}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{2946FB2A-71EE-4D66-8EE3-C8A44FDB6146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F44407A8-F22C-4383-9374-2B3CF61AF790}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="740" windowWidth="19180" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -832,6 +832,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1100,8 +1104,8 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>